<commit_message>
Introduce new way of AI cheating
Pros:
Better AI performance on Deity
AI players will have less cash so human players can't exploit them
AI's city looks more "realistic" (without inflated yields)
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078C2CF6-151C-45DD-B752-878348C6B070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C9CE58-917E-469C-ADE0-A46797D58F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2832" yWindow="0" windowWidth="19500" windowHeight="11688" xr2:uid="{E8AAC43B-5A54-406D-B95D-5DF386335546}"/>
   </bookViews>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E97-52CE-4D75-8992-93CFC5B46B46}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1037,23 +1037,23 @@
         <v>1.5</v>
       </c>
       <c r="C18">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="D18">
         <v>1.4</v>
       </c>
       <c r="E18">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="F18">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="G18">
         <v>0.75</v>
       </c>
       <c r="H18">
         <f>SUM(B18:G18)</f>
-        <v>7.1499999999999995</v>
+        <v>7.3</v>
       </c>
       <c r="J18">
         <f>B18-1</f>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="K18">
         <f t="shared" ref="K18:O18" si="12">C18-1</f>
-        <v>0.10000000000000009</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="L18">
         <f t="shared" si="12"/>
@@ -1069,11 +1069,11 @@
       </c>
       <c r="M18">
         <f t="shared" si="12"/>
-        <v>0.10000000000000009</v>
+        <v>0.25</v>
       </c>
       <c r="N18">
         <f t="shared" si="12"/>
-        <v>0.30000000000000004</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="O18">
         <f t="shared" si="12"/>
@@ -1088,23 +1088,23 @@
         <v>1.6</v>
       </c>
       <c r="C19">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="D19">
         <v>1.45</v>
       </c>
       <c r="E19">
-        <v>1.1000000000000001</v>
+        <v>1.35</v>
       </c>
       <c r="F19">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="G19">
         <v>0.75</v>
       </c>
       <c r="H19">
         <f t="shared" ref="H19:H23" si="13">SUM(B19:G19)</f>
-        <v>7.5</v>
+        <v>7.7500000000000009</v>
       </c>
       <c r="J19">
         <f>B19-B18</f>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="K19">
         <f t="shared" ref="K19:O23" si="14">C19-C18</f>
-        <v>9.9999999999999867E-2</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="L19">
         <f t="shared" si="14"/>
@@ -1120,11 +1120,11 @@
       </c>
       <c r="M19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="N19">
         <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="O19">
         <f t="shared" si="14"/>
@@ -1145,7 +1145,7 @@
         <v>1.5</v>
       </c>
       <c r="E20">
-        <v>1.2</v>
+        <v>1.45</v>
       </c>
       <c r="F20">
         <v>1.2</v>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="13"/>
-        <v>7.6000000000000005</v>
+        <v>7.8500000000000005</v>
       </c>
       <c r="J20">
         <f t="shared" ref="J20:J23" si="15">B20-B19</f>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="14"/>
-        <v>0.40000000000000013</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="L20">
         <f t="shared" si="14"/>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="14"/>
-        <v>-0.19999999999999996</v>
+        <v>-0.10000000000000009</v>
       </c>
       <c r="O20">
         <f t="shared" si="14"/>
@@ -1196,7 +1196,7 @@
         <v>1.7</v>
       </c>
       <c r="E21">
-        <v>1.2</v>
+        <v>1.55</v>
       </c>
       <c r="F21">
         <v>1.1000000000000001</v>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="13"/>
-        <v>7.7</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="J21">
         <f t="shared" si="15"/>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="M21">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="N21">
         <f t="shared" si="14"/>
@@ -1247,7 +1247,7 @@
         <v>1.75</v>
       </c>
       <c r="E22">
-        <v>1.2</v>
+        <v>1.65</v>
       </c>
       <c r="F22">
         <v>1.1000000000000001</v>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="13"/>
-        <v>7.8</v>
+        <v>8.25</v>
       </c>
       <c r="J22">
         <f t="shared" si="15"/>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>9.9999999999999867E-2</v>
       </c>
       <c r="N22">
         <f t="shared" si="14"/>
@@ -1298,7 +1298,7 @@
         <v>1.75</v>
       </c>
       <c r="E23">
-        <v>1.2</v>
+        <v>1.75</v>
       </c>
       <c r="F23">
         <v>1.1000000000000001</v>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="13"/>
-        <v>8.0000000000000018</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="J23">
         <f t="shared" si="15"/>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="M23">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="N23">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
Sistine is an AI tweak mod (I'm sure)
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C9CE58-917E-469C-ADE0-A46797D58F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFD6D3B-2B01-4051-B4DC-E5D199B14BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2832" yWindow="0" windowWidth="19500" windowHeight="11688" xr2:uid="{E8AAC43B-5A54-406D-B95D-5DF386335546}"/>
+    <workbookView xWindow="-96" yWindow="6120" windowWidth="23184" windowHeight="6216" xr2:uid="{E8AAC43B-5A54-406D-B95D-5DF386335546}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E97-52CE-4D75-8992-93CFC5B46B46}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1094,7 @@
         <v>1.45</v>
       </c>
       <c r="E19">
-        <v>1.35</v>
+        <v>1.4</v>
       </c>
       <c r="F19">
         <v>1.3</v>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="H19">
         <f t="shared" ref="H19:H23" si="13">SUM(B19:G19)</f>
-        <v>7.7500000000000009</v>
+        <v>7.8</v>
       </c>
       <c r="J19">
         <f>B19-B18</f>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="M19">
         <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
+        <v>0.14999999999999991</v>
       </c>
       <c r="N19">
         <f t="shared" si="14"/>
@@ -1145,7 +1145,7 @@
         <v>1.5</v>
       </c>
       <c r="E20">
-        <v>1.45</v>
+        <v>1.55</v>
       </c>
       <c r="F20">
         <v>1.2</v>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="13"/>
-        <v>7.8500000000000005</v>
+        <v>7.95</v>
       </c>
       <c r="J20">
         <f t="shared" ref="J20:J23" si="15">B20-B19</f>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="M20">
         <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
+        <v>0.15000000000000013</v>
       </c>
       <c r="N20">
         <f t="shared" si="14"/>
@@ -1193,13 +1193,13 @@
         <v>1.7</v>
       </c>
       <c r="D21">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="E21">
-        <v>1.55</v>
+        <v>1.6</v>
       </c>
       <c r="F21">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G21">
         <v>0.3</v>
@@ -1218,15 +1218,15 @@
       </c>
       <c r="L21">
         <f t="shared" si="14"/>
-        <v>0.19999999999999996</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="M21">
         <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="N21">
         <f t="shared" si="14"/>
-        <v>-9.9999999999999867E-2</v>
+        <v>-5.0000000000000044E-2</v>
       </c>
       <c r="O21">
         <f t="shared" si="14"/>
@@ -1244,20 +1244,20 @@
         <v>1.75</v>
       </c>
       <c r="D22">
+        <v>1.7</v>
+      </c>
+      <c r="E22">
         <v>1.75</v>
       </c>
-      <c r="E22">
-        <v>1.65</v>
-      </c>
       <c r="F22">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G22">
         <v>0.3</v>
       </c>
       <c r="H22">
         <f t="shared" si="13"/>
-        <v>8.25</v>
+        <v>8.3500000000000014</v>
       </c>
       <c r="J22">
         <f t="shared" si="15"/>
@@ -1269,11 +1269,11 @@
       </c>
       <c r="L22">
         <f t="shared" si="14"/>
-        <v>5.0000000000000044E-2</v>
+        <v>9.9999999999999867E-2</v>
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
+        <v>0.14999999999999991</v>
       </c>
       <c r="N22">
         <f t="shared" si="14"/>
@@ -1289,10 +1289,10 @@
         <v>11</v>
       </c>
       <c r="B23">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="C23">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="D23">
         <v>1.75</v>
@@ -1301,7 +1301,7 @@
         <v>1.75</v>
       </c>
       <c r="F23">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G23">
         <v>0.3</v>
@@ -1312,19 +1312,19 @@
       </c>
       <c r="J23">
         <f t="shared" si="15"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="14"/>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="14"/>
-        <v>0.14999999999999991</v>
-      </c>
       <c r="L23">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="M23">
         <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
+        <v>0</v>
       </c>
       <c r="N23">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
AI weight update (again)
We dedicate ourselves in improving AI so extremely that we nearly forgot that we still have plans to do!
But, you know, if it doesn't work well on AI, players won't be happy.
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFD6D3B-2B01-4051-B4DC-E5D199B14BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4D0659-0E92-4A0B-A1D9-5254BAABF916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="6120" windowWidth="23184" windowHeight="6216" xr2:uid="{E8AAC43B-5A54-406D-B95D-5DF386335546}"/>
+    <workbookView xWindow="2832" yWindow="0" windowWidth="19500" windowHeight="11688" xr2:uid="{E8AAC43B-5A54-406D-B95D-5DF386335546}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E97-52CE-4D75-8992-93CFC5B46B46}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1145,17 +1145,17 @@
         <v>1.5</v>
       </c>
       <c r="E20">
-        <v>1.55</v>
+        <v>1.5</v>
       </c>
       <c r="F20">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>0.5</v>
       </c>
       <c r="H20">
         <f t="shared" si="13"/>
-        <v>7.95</v>
+        <v>7.7</v>
       </c>
       <c r="J20">
         <f t="shared" ref="J20:J23" si="15">B20-B19</f>
@@ -1171,11 +1171,11 @@
       </c>
       <c r="M20">
         <f t="shared" si="14"/>
-        <v>0.15000000000000013</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="N20">
         <f t="shared" si="14"/>
-        <v>-0.10000000000000009</v>
+        <v>-0.30000000000000004</v>
       </c>
       <c r="O20">
         <f t="shared" si="14"/>
@@ -1196,17 +1196,17 @@
         <v>1.6</v>
       </c>
       <c r="E21">
-        <v>1.6</v>
+        <v>1.55</v>
       </c>
       <c r="F21">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>0.3</v>
       </c>
       <c r="H21">
         <f t="shared" si="13"/>
-        <v>8.0500000000000007</v>
+        <v>7.85</v>
       </c>
       <c r="J21">
         <f t="shared" si="15"/>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="N21">
         <f t="shared" si="14"/>
-        <v>-5.0000000000000044E-2</v>
+        <v>0</v>
       </c>
       <c r="O21">
         <f t="shared" si="14"/>
@@ -1247,17 +1247,17 @@
         <v>1.7</v>
       </c>
       <c r="E22">
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
       <c r="F22">
-        <v>1.1499999999999999</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>0.3</v>
       </c>
       <c r="H22">
         <f t="shared" si="13"/>
-        <v>8.3500000000000014</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="J22">
         <f t="shared" si="15"/>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
-        <v>0.14999999999999991</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="N22">
         <f t="shared" si="14"/>
@@ -1298,17 +1298,17 @@
         <v>1.75</v>
       </c>
       <c r="E23">
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
       <c r="F23">
-        <v>1.1499999999999999</v>
+        <v>0.9</v>
       </c>
       <c r="G23">
         <v>0.3</v>
       </c>
       <c r="H23">
         <f t="shared" si="13"/>
-        <v>8.5500000000000007</v>
+        <v>8.15</v>
       </c>
       <c r="J23">
         <f t="shared" si="15"/>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="N23">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-9.9999999999999978E-2</v>
       </c>
       <c r="O23">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
[WIP] New AI changes
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4D0659-0E92-4A0B-A1D9-5254BAABF916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EAA18F-EB7F-4B78-885A-BD84C60D2762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2832" yWindow="0" windowWidth="19500" windowHeight="11688" xr2:uid="{E8AAC43B-5A54-406D-B95D-5DF386335546}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1046,14 +1046,14 @@
         <v>1.25</v>
       </c>
       <c r="F18">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0.75</v>
       </c>
       <c r="H18">
         <f>SUM(B18:G18)</f>
-        <v>7.3</v>
+        <v>7.1</v>
       </c>
       <c r="J18">
         <f>B18-1</f>
@@ -1073,7 +1073,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="12"/>
-        <v>0.19999999999999996</v>
+        <v>0</v>
       </c>
       <c r="O18">
         <f t="shared" si="12"/>
@@ -1097,14 +1097,14 @@
         <v>1.4</v>
       </c>
       <c r="F19">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0.75</v>
       </c>
       <c r="H19">
         <f t="shared" ref="H19:H23" si="13">SUM(B19:G19)</f>
-        <v>7.8</v>
+        <v>7.5</v>
       </c>
       <c r="J19">
         <f>B19-B18</f>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="N19">
         <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <f t="shared" si="14"/>
@@ -1148,14 +1148,14 @@
         <v>1.5</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G20">
         <v>0.5</v>
       </c>
       <c r="H20">
         <f t="shared" si="13"/>
-        <v>7.7</v>
+        <v>7.2</v>
       </c>
       <c r="J20">
         <f t="shared" ref="J20:J23" si="15">B20-B19</f>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="14"/>
-        <v>-0.30000000000000004</v>
+        <v>-0.5</v>
       </c>
       <c r="O20">
         <f t="shared" si="14"/>
@@ -1199,14 +1199,14 @@
         <v>1.55</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G21">
         <v>0.3</v>
       </c>
       <c r="H21">
         <f t="shared" si="13"/>
-        <v>7.85</v>
+        <v>7.35</v>
       </c>
       <c r="J21">
         <f t="shared" si="15"/>
@@ -1250,14 +1250,14 @@
         <v>1.6</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="G22">
         <v>0.3</v>
       </c>
       <c r="H22">
         <f t="shared" si="13"/>
-        <v>8.0500000000000007</v>
+        <v>7.35</v>
       </c>
       <c r="J22">
         <f t="shared" si="15"/>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="N22">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="O22">
         <f t="shared" si="14"/>
@@ -1301,14 +1301,14 @@
         <v>1.6</v>
       </c>
       <c r="F23">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="G23">
         <v>0.3</v>
       </c>
       <c r="H23">
         <f t="shared" si="13"/>
-        <v>8.15</v>
+        <v>7.5499999999999989</v>
       </c>
       <c r="J23">
         <f t="shared" si="15"/>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="N23">
         <f t="shared" si="14"/>
-        <v>-9.9999999999999978E-2</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
[TESTING] Temporarily revert AI cheat and try to consider Prince difficulty
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12540"/>
+    <workbookView windowWidth="28050" windowHeight="5550"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1002,8 +1002,8 @@
   <sheetPr/>
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1571,7 +1571,7 @@
         <v>7</v>
       </c>
       <c r="B18">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="C18">
         <v>1.2</v>
@@ -1583,7 +1583,7 @@
         <v>1.25</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="G18">
         <v>0.75</v>
@@ -1594,7 +1594,7 @@
       </c>
       <c r="J18">
         <f>B18-1</f>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="K18">
         <f t="shared" ref="K18:O18" si="12">C18-1</f>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="O18">
         <f t="shared" si="12"/>
@@ -1622,7 +1622,7 @@
         <v>8</v>
       </c>
       <c r="B19">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="C19">
         <v>1.3</v>
@@ -1641,11 +1641,11 @@
       </c>
       <c r="H19">
         <f t="shared" ref="H19:H23" si="13">SUM(B19:G19)</f>
-        <v>7.5</v>
+        <v>7.4</v>
       </c>
       <c r="J19">
         <f>B19-B18</f>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="K19">
         <f t="shared" ref="K19:O23" si="14">C19-C18</f>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="N19">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-0.2</v>
       </c>
       <c r="O19">
         <f t="shared" si="14"/>
@@ -1685,18 +1685,18 @@
         <v>1.5</v>
       </c>
       <c r="F20">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="G20">
         <v>0.5</v>
       </c>
       <c r="H20">
         <f t="shared" si="13"/>
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
       <c r="J20">
         <f t="shared" ref="J20:J23" si="15">B20-B19</f>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="K20">
         <f t="shared" si="14"/>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="14"/>
-        <v>-0.4</v>
+        <v>-0.3</v>
       </c>
       <c r="O20">
         <f t="shared" si="14"/>
@@ -1733,17 +1733,17 @@
         <v>1.6</v>
       </c>
       <c r="E21">
-        <v>1.55</v>
+        <v>1.6</v>
       </c>
       <c r="F21">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="G21">
         <v>0.3</v>
       </c>
       <c r="H21">
         <f t="shared" si="13"/>
-        <v>7.25</v>
+        <v>7.5</v>
       </c>
       <c r="J21">
         <f t="shared" si="15"/>
@@ -1759,11 +1759,11 @@
       </c>
       <c r="M21">
         <f t="shared" si="14"/>
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="N21">
         <f t="shared" si="14"/>
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="O21">
         <f t="shared" si="14"/>
@@ -1787,14 +1787,14 @@
         <v>1.6</v>
       </c>
       <c r="F22">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="G22">
         <v>0.3</v>
       </c>
       <c r="H22">
         <f t="shared" si="13"/>
-        <v>7.45</v>
+        <v>7.55</v>
       </c>
       <c r="J22">
         <f t="shared" si="15"/>
@@ -1810,11 +1810,11 @@
       </c>
       <c r="M22">
         <f t="shared" si="14"/>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="N22">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="O22">
         <f t="shared" si="14"/>
@@ -1835,17 +1835,17 @@
         <v>1.75</v>
       </c>
       <c r="E23">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="F23">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G23">
         <v>0.3</v>
       </c>
       <c r="H23">
         <f t="shared" si="13"/>
-        <v>7.55</v>
+        <v>7.75</v>
       </c>
       <c r="J23">
         <f t="shared" si="15"/>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="M23">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.0999999999999999</v>
       </c>
       <c r="N23">
         <f t="shared" si="14"/>

</xml_diff>

<commit_message>
Partially revert reduced Food weight
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60FC777-0B9F-425C-BA8A-2837862BE834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EAA965-9FC4-4327-B922-9EFC0F67A694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="552" windowWidth="19500" windowHeight="11688" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1139,14 +1139,14 @@
         <v>1.6</v>
       </c>
       <c r="F21">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="G21">
         <v>0.3</v>
       </c>
       <c r="H21">
         <f t="shared" si="13"/>
-        <v>7.7</v>
+        <v>7.8000000000000007</v>
       </c>
       <c r="J21">
         <f t="shared" si="15"/>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="N21">
         <f t="shared" si="14"/>
-        <v>-9.9999999999999978E-2</v>
+        <v>0</v>
       </c>
       <c r="O21">
         <f t="shared" si="14"/>
@@ -1190,14 +1190,14 @@
         <v>1.6</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G22">
         <v>0.3</v>
       </c>
       <c r="H22">
         <f t="shared" si="13"/>
-        <v>7.8999999999999995</v>
+        <v>8.1</v>
       </c>
       <c r="J22">
         <f t="shared" si="15"/>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="N22">
         <f t="shared" si="14"/>
-        <v>-9.9999999999999978E-2</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <f t="shared" si="14"/>
@@ -1241,14 +1241,14 @@
         <v>1.7</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G23">
         <v>0.3</v>
       </c>
       <c r="H23">
         <f t="shared" si="13"/>
-        <v>8.1999999999999993</v>
+        <v>8.4</v>
       </c>
       <c r="J23">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
Trials on AI perf
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94734784-DE0F-40C0-BE94-279AB4ABF63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8505DD27-EB3B-4E02-8863-96763AF0557C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16440" yWindow="2970" windowWidth="19620" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="16">
-  <si>
-    <t>假设进入新时代将会抛弃旧时代策略</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
   <si>
     <t>锤</t>
   </si>
@@ -74,20 +71,21 @@
     <t>现代（电气以后）</t>
   </si>
   <si>
-    <t>假设进入新时代不会抛弃旧时代策略</t>
-  </si>
-  <si>
     <t>delta</t>
   </si>
   <si>
     <t>理想</t>
+  </si>
+  <si>
+    <t>原版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +96,14 @@
     <font>
       <sz val="9"/>
       <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -124,8 +130,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -415,31 +424,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1.25</v>
@@ -459,10 +489,38 @@
       <c r="G2">
         <v>0.75</v>
       </c>
+      <c r="H2">
+        <f>SUM(B2:G2)</f>
+        <v>6.4</v>
+      </c>
+      <c r="J2">
+        <f>B2-1</f>
+        <v>0.25</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2" si="0">C2-1</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2" si="1">D2-1</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2" si="2">E2-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2" si="3">F2-1</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ref="O2" si="4">G2-1</f>
+        <v>-0.25</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1.25</v>
@@ -482,97 +540,237 @@
       <c r="G3">
         <v>0.95</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="5">SUM(B3:G3)</f>
+        <v>7.3000000000000007</v>
+      </c>
+      <c r="J3">
+        <f>B3-B2</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K7" si="6">C3-C2</f>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L7" si="7">D3-D2</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M7" si="8">E3-E2</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N7" si="9">F3-F2</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O7" si="10">G3-G2</f>
+        <v>0.19999999999999996</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1.25</v>
       </c>
       <c r="C4">
-        <v>1.25</v>
+        <v>1.55</v>
       </c>
       <c r="D4">
         <v>1.1000000000000001</v>
       </c>
       <c r="E4">
-        <v>1.35</v>
+        <v>1.55</v>
       </c>
       <c r="F4">
-        <v>1.25</v>
+        <v>1.45</v>
       </c>
       <c r="G4">
-        <v>0.5</v>
+        <v>0.7</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="5"/>
+        <v>7.6000000000000005</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J7" si="11">B4-B3</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="6"/>
+        <v>0.15000000000000013</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="8"/>
+        <v>0.15000000000000013</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="9"/>
+        <v>0.25</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="10"/>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>1.25</v>
       </c>
       <c r="C5">
-        <v>1.1000000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="D5">
         <v>1.1000000000000001</v>
       </c>
       <c r="E5">
-        <v>1.35</v>
+        <v>1.7</v>
       </c>
       <c r="F5">
-        <v>1.1000000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="G5">
-        <v>0.75</v>
+        <v>0.7</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="5"/>
+        <v>7.85</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="8"/>
+        <v>0.14999999999999991</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="9"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>1.25</v>
       </c>
       <c r="C6">
-        <v>1.1000000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="D6">
         <v>1.1000000000000001</v>
       </c>
       <c r="E6">
-        <v>1.35</v>
+        <v>1.85</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>1.55</v>
       </c>
       <c r="G6">
-        <v>0.35</v>
+        <v>0.3</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="5"/>
+        <v>7.6</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="8"/>
+        <v>0.15000000000000013</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="10"/>
+        <v>-0.39999999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>1.25</v>
       </c>
       <c r="C7">
-        <v>1.1000000000000001</v>
+        <v>1.55</v>
       </c>
       <c r="D7">
         <v>1.1000000000000001</v>
       </c>
       <c r="E7">
-        <v>1.3</v>
+        <v>1.95</v>
       </c>
       <c r="F7">
-        <v>1.05</v>
+        <v>1.6</v>
       </c>
       <c r="G7">
-        <v>0.75</v>
+        <v>0.3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="5"/>
+        <v>7.7499999999999991</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="8"/>
+        <v>9.9999999999999867E-2</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="9"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -580,697 +778,347 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>4</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>5</v>
       </c>
-      <c r="G9" t="s">
-        <v>6</v>
-      </c>
       <c r="I9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J9" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
         <v>1</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>2</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>3</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>4</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>5</v>
-      </c>
-      <c r="O9" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>1.25</v>
+        <v>1.3</v>
       </c>
       <c r="C10">
         <v>1.1000000000000001</v>
       </c>
       <c r="D10">
-        <v>1.1000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="E10">
         <v>1.2</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="G10">
         <v>0.75</v>
       </c>
       <c r="H10">
         <f>SUM(B10:G10)</f>
-        <v>6.4</v>
+        <v>6.95</v>
       </c>
       <c r="J10">
         <f>B10-1</f>
-        <v>0.25</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K10" si="0">C10-1</f>
+        <f t="shared" ref="K10:O10" si="12">C10-1</f>
         <v>0.10000000000000009</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10" si="1">D10-1</f>
-        <v>0.10000000000000009</v>
+        <f t="shared" si="12"/>
+        <v>0.39999999999999991</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10" si="2">E10-1</f>
+        <f t="shared" si="12"/>
         <v>0.19999999999999996</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10" si="3">F10-1</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>0.19999999999999996</v>
       </c>
       <c r="O10">
-        <f t="shared" ref="O10" si="4">G10-1</f>
+        <f t="shared" si="12"/>
         <v>-0.25</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="C11">
         <v>1.4</v>
       </c>
       <c r="D11">
-        <v>1.1000000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="E11">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="F11">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0.95</v>
+        <v>0.75</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:H15" si="5">SUM(B11:G11)</f>
-        <v>7.3000000000000007</v>
+        <f t="shared" ref="H11:H15" si="13">SUM(B11:G11)</f>
+        <v>7.35</v>
       </c>
       <c r="J11">
         <f>B11-B10</f>
-        <v>0</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11:K15" si="6">C11-C10</f>
+        <f t="shared" ref="K11:O15" si="14">C11-C10</f>
         <v>0.29999999999999982</v>
       </c>
       <c r="L11">
-        <f t="shared" ref="L11:L15" si="7">D11-D10</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M11:M15" si="8">E11-E10</f>
-        <v>0.19999999999999996</v>
+        <f t="shared" si="14"/>
+        <v>0.10000000000000009</v>
       </c>
       <c r="N11">
-        <f t="shared" ref="N11:N15" si="9">F11-F10</f>
-        <v>0.19999999999999996</v>
+        <f t="shared" si="14"/>
+        <v>-0.19999999999999996</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:O15" si="10">G11-G10</f>
-        <v>0.19999999999999996</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>1.25</v>
+        <v>1.7</v>
       </c>
       <c r="C12">
-        <v>1.55</v>
+        <v>1.7</v>
       </c>
       <c r="D12">
-        <v>1.1000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="E12">
-        <v>1.55</v>
+        <v>1.5</v>
       </c>
       <c r="F12">
-        <v>1.45</v>
+        <v>0.7</v>
       </c>
       <c r="G12">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H12">
-        <f t="shared" si="5"/>
-        <v>7.6000000000000005</v>
+        <f t="shared" si="13"/>
+        <v>7.7</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J15" si="11">B12-B11</f>
-        <v>0</v>
+        <f t="shared" ref="J12:J15" si="15">B12-B11</f>
+        <v>0.19999999999999996</v>
       </c>
       <c r="K12">
-        <f t="shared" si="6"/>
-        <v>0.15000000000000013</v>
+        <f t="shared" si="14"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="L12">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.20000000000000018</v>
       </c>
       <c r="M12">
-        <f t="shared" si="8"/>
-        <v>0.15000000000000013</v>
+        <f t="shared" si="14"/>
+        <v>0.19999999999999996</v>
       </c>
       <c r="N12">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
+        <f t="shared" si="14"/>
+        <v>-0.30000000000000004</v>
       </c>
       <c r="O12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-0.25</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>1.25</v>
+        <v>1.8</v>
       </c>
       <c r="C13">
-        <v>1.55</v>
+        <v>1.8</v>
       </c>
       <c r="D13">
-        <v>1.1000000000000001</v>
+        <v>1.7</v>
       </c>
       <c r="E13">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="F13">
-        <v>1.55</v>
+        <v>0.7</v>
       </c>
       <c r="G13">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="H13">
-        <f t="shared" si="5"/>
-        <v>7.85</v>
+        <f t="shared" si="13"/>
+        <v>7.9</v>
       </c>
       <c r="J13">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>0.10000000000000009</v>
       </c>
       <c r="K13">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.10000000000000009</v>
       </c>
       <c r="L13">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>9.9999999999999867E-2</v>
       </c>
       <c r="M13">
-        <f t="shared" si="8"/>
-        <v>0.14999999999999991</v>
+        <f t="shared" si="14"/>
+        <v>0.10000000000000009</v>
       </c>
       <c r="N13">
-        <f t="shared" si="9"/>
-        <v>0.10000000000000009</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14">
-        <v>1.25</v>
+        <v>1.8</v>
       </c>
       <c r="C14">
-        <v>1.55</v>
+        <v>1.9</v>
       </c>
       <c r="D14">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="E14">
-        <v>1.85</v>
+        <v>1.6</v>
       </c>
       <c r="F14">
-        <v>1.55</v>
+        <v>0.7</v>
       </c>
       <c r="G14">
         <v>0.3</v>
       </c>
       <c r="H14">
-        <f t="shared" si="5"/>
-        <v>7.6</v>
+        <f t="shared" si="13"/>
+        <v>8.1</v>
       </c>
       <c r="J14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="K14">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>9.9999999999999867E-2</v>
       </c>
       <c r="L14">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.10000000000000009</v>
       </c>
       <c r="M14">
-        <f t="shared" si="8"/>
-        <v>0.15000000000000013</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="10"/>
-        <v>-0.39999999999999997</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>1.55</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>1.1000000000000001</v>
+        <v>1.8</v>
       </c>
       <c r="E15">
-        <v>1.95</v>
+        <v>1.7</v>
       </c>
       <c r="F15">
-        <v>1.6</v>
+        <v>0.7</v>
       </c>
       <c r="G15">
         <v>0.3</v>
       </c>
       <c r="H15">
-        <f t="shared" si="5"/>
-        <v>7.7499999999999991</v>
+        <f t="shared" si="13"/>
+        <v>8.5</v>
       </c>
       <c r="J15">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>0.19999999999999996</v>
       </c>
       <c r="K15">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>0.10000000000000009</v>
       </c>
       <c r="L15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="14"/>
         <v>9.9999999999999867E-2</v>
       </c>
       <c r="N15">
-        <f t="shared" si="9"/>
-        <v>5.0000000000000044E-2</v>
+        <f t="shared" si="14"/>
+        <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1</v>
-      </c>
-      <c r="K17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" t="s">
-        <v>3</v>
-      </c>
-      <c r="M17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N17" t="s">
-        <v>5</v>
-      </c>
-      <c r="O17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18">
-        <v>1.3</v>
-      </c>
-      <c r="C18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D18">
-        <v>1.4</v>
-      </c>
-      <c r="E18">
-        <v>1.2</v>
-      </c>
-      <c r="F18">
-        <v>1.2</v>
-      </c>
-      <c r="G18">
-        <v>0.75</v>
-      </c>
-      <c r="H18">
-        <f>SUM(B18:G18)</f>
-        <v>6.95</v>
-      </c>
-      <c r="J18">
-        <f>B18-1</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="K18">
-        <f t="shared" ref="K18:O18" si="12">C18-1</f>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="12"/>
-        <v>0.39999999999999991</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="12"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="N18">
-        <f t="shared" si="12"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="12"/>
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19">
-        <v>1.5</v>
-      </c>
-      <c r="C19">
-        <v>1.4</v>
-      </c>
-      <c r="D19">
-        <v>1.4</v>
-      </c>
-      <c r="E19">
-        <v>1.3</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>0.75</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ref="H19:H23" si="13">SUM(B19:G19)</f>
-        <v>7.35</v>
-      </c>
-      <c r="J19">
-        <f>B19-B18</f>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="K19">
-        <f t="shared" ref="K19:O23" si="14">C19-C18</f>
-        <v>0.29999999999999982</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="N19">
-        <f t="shared" si="14"/>
-        <v>-0.19999999999999996</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20">
-        <v>1.7</v>
-      </c>
-      <c r="C20">
-        <v>1.7</v>
-      </c>
-      <c r="D20">
-        <v>1.6</v>
-      </c>
-      <c r="E20">
-        <v>1.5</v>
-      </c>
-      <c r="F20">
-        <v>0.7</v>
-      </c>
-      <c r="G20">
-        <v>0.5</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="13"/>
-        <v>7.7</v>
-      </c>
-      <c r="J20">
-        <f t="shared" ref="J20:J23" si="15">B20-B19</f>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="14"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="14"/>
-        <v>0.20000000000000018</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="14"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="N20">
-        <f t="shared" si="14"/>
-        <v>-0.30000000000000004</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="14"/>
-        <v>-0.25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21">
-        <v>1.7</v>
-      </c>
-      <c r="C21">
-        <v>1.8</v>
-      </c>
-      <c r="D21">
-        <v>1.7</v>
-      </c>
-      <c r="E21">
-        <v>1.6</v>
-      </c>
-      <c r="F21">
-        <v>0.7</v>
-      </c>
-      <c r="G21">
-        <v>0.3</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="13"/>
-        <v>7.8000000000000007</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="N21">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="14"/>
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22">
-        <v>1.8</v>
-      </c>
-      <c r="C22">
-        <v>1.9</v>
-      </c>
-      <c r="D22">
-        <v>1.8</v>
-      </c>
-      <c r="E22">
-        <v>1.6</v>
-      </c>
-      <c r="F22">
-        <v>0.7</v>
-      </c>
-      <c r="G22">
-        <v>0.3</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="13"/>
-        <v>8.1</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="15"/>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23">
-        <v>1.8</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
-        <v>1.9</v>
-      </c>
-      <c r="E23">
-        <v>1.7</v>
-      </c>
-      <c r="F23">
-        <v>0.7</v>
-      </c>
-      <c r="G23">
-        <v>0.3</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="13"/>
-        <v>8.4</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="O23">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Some power! for AI
At least when we were testing it...
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8505DD27-EB3B-4E02-8863-96763AF0557C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3854FE-EF39-47CB-AACD-0315E12F6493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16440" yWindow="2970" windowWidth="19620" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>锤</t>
   </si>
@@ -78,6 +78,10 @@
   </si>
   <si>
     <t>原版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -412,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -825,10 +829,10 @@
         <v>1.3</v>
       </c>
       <c r="C10">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="D10">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E10">
         <v>1.2</v>
@@ -849,11 +853,11 @@
       </c>
       <c r="K10">
         <f t="shared" ref="K10:O10" si="12">C10-1</f>
-        <v>0.10000000000000009</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="L10">
         <f t="shared" si="12"/>
-        <v>0.39999999999999991</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="M10">
         <f t="shared" si="12"/>
@@ -879,7 +883,7 @@
         <v>1.4</v>
       </c>
       <c r="D11">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E11">
         <v>1.3</v>
@@ -892,15 +896,15 @@
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H15" si="13">SUM(B11:G11)</f>
-        <v>7.35</v>
+        <v>7.25</v>
       </c>
       <c r="J11">
         <f>B11-B10</f>
         <v>0.19999999999999996</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11:O15" si="14">C11-C10</f>
-        <v>0.29999999999999982</v>
+        <f t="shared" ref="J11:O16" si="14">C11-C10</f>
+        <v>0.19999999999999996</v>
       </c>
       <c r="L11">
         <f t="shared" si="14"/>
@@ -930,7 +934,7 @@
         <v>1.7</v>
       </c>
       <c r="D12">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E12">
         <v>1.5</v>
@@ -943,7 +947,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="13"/>
-        <v>7.7</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="J12">
         <f t="shared" ref="J12:J15" si="15">B12-B11</f>
@@ -955,7 +959,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="14"/>
-        <v>0.20000000000000018</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="M12">
         <f t="shared" si="14"/>
@@ -978,10 +982,10 @@
         <v>1.8</v>
       </c>
       <c r="C13">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="E13">
         <v>1.6</v>
@@ -994,7 +998,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="13"/>
-        <v>7.9</v>
+        <v>8</v>
       </c>
       <c r="J13">
         <f t="shared" si="15"/>
@@ -1002,11 +1006,11 @@
       </c>
       <c r="K13">
         <f t="shared" si="14"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="14"/>
         <v>0.10000000000000009</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="14"/>
-        <v>9.9999999999999867E-2</v>
       </c>
       <c r="M13">
         <f t="shared" si="14"/>
@@ -1029,10 +1033,10 @@
         <v>1.8</v>
       </c>
       <c r="C14">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="D14">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="E14">
         <v>1.6</v>
@@ -1045,7 +1049,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="13"/>
-        <v>8.1</v>
+        <v>8.6</v>
       </c>
       <c r="J14">
         <f t="shared" si="15"/>
@@ -1053,11 +1057,11 @@
       </c>
       <c r="K14">
         <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="14"/>
         <v>9.9999999999999867E-2</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="14"/>
-        <v>0.10000000000000009</v>
       </c>
       <c r="M14">
         <f t="shared" si="14"/>
@@ -1080,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D15">
         <v>1.8</v>
@@ -1096,7 +1100,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="13"/>
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="J15">
         <f t="shared" si="15"/>
@@ -1104,12 +1108,12 @@
       </c>
       <c r="K15">
         <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="14"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
       <c r="M15">
         <f t="shared" si="14"/>
         <v>9.9999999999999867E-2</v>
@@ -1121,6 +1125,25 @@
       <c r="O15">
         <f t="shared" si="14"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2.5</v>
+      </c>
+      <c r="C16">
+        <v>1.8</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="14"/>
+        <v>0.5</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="14"/>
+        <v>-0.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make science building earlier
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3854FE-EF39-47CB-AACD-0315E12F6493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52241232-152B-4E76-8F02-C4D84DA6B823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="3180" windowWidth="19620" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -931,7 +931,7 @@
         <v>1.7</v>
       </c>
       <c r="C12">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>1.5</v>
@@ -947,7 +947,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="13"/>
-        <v>7.6000000000000005</v>
+        <v>7.9</v>
       </c>
       <c r="J12">
         <f t="shared" ref="J12:J15" si="15">B12-B11</f>
@@ -955,7 +955,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="14"/>
-        <v>0.30000000000000004</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="L12">
         <f t="shared" si="14"/>
@@ -982,7 +982,7 @@
         <v>1.8</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D13">
         <v>1.6</v>
@@ -998,7 +998,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="13"/>
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="J13">
         <f t="shared" si="15"/>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="14"/>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="L13">
         <f t="shared" si="14"/>
@@ -1030,7 +1030,7 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>2.5</v>
@@ -1049,15 +1049,15 @@
       </c>
       <c r="H14">
         <f t="shared" si="13"/>
-        <v>8.6</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J14">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="K14">
         <f t="shared" si="14"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="L14">
         <f t="shared" si="14"/>
@@ -1084,7 +1084,7 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>1.8</v>
@@ -1100,15 +1100,15 @@
       </c>
       <c r="H15">
         <f t="shared" si="13"/>
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="J15">
         <f t="shared" si="15"/>
-        <v>0.19999999999999996</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="L15">
         <f t="shared" si="14"/>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="14"/>
-        <v>-0.7</v>
+        <v>-0.19999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
readjust ai yield weight
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52241232-152B-4E76-8F02-C4D84DA6B823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73505924-A307-450C-9AEB-C24ECD48AF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="3180" windowWidth="19620" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1081,10 +1081,10 @@
         <v>11</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D15">
         <v>1.8</v>
@@ -1093,22 +1093,22 @@
         <v>1.7</v>
       </c>
       <c r="F15">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="G15">
         <v>0.3</v>
       </c>
       <c r="H15">
         <f t="shared" si="13"/>
-        <v>8.5</v>
+        <v>8.9</v>
       </c>
       <c r="J15">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>0.20000000000000018</v>
       </c>
       <c r="K15">
         <f t="shared" si="14"/>
-        <v>-0.5</v>
+        <v>-0.20000000000000018</v>
       </c>
       <c r="L15">
         <f t="shared" si="14"/>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>-9.9999999999999978E-2</v>
       </c>
       <c r="O15">
         <f t="shared" si="14"/>
@@ -1135,15 +1135,15 @@
         <v>2.5</v>
       </c>
       <c r="C16">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="J16">
         <f t="shared" si="14"/>
-        <v>0.5</v>
+        <v>0.29999999999999982</v>
       </c>
       <c r="K16">
         <f t="shared" si="14"/>
-        <v>-0.19999999999999996</v>
+        <v>-0.29999999999999982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Slightly ramp up food weight
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F86627A-EEF3-4E6B-95D8-01C9DB17BFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB13E3A4-181C-467C-9A31-DDFF72B92EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9855" yWindow="2655" windowWidth="27915" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="2940" windowWidth="26205" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -889,14 +889,14 @@
         <v>1.3</v>
       </c>
       <c r="F11">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="G11">
         <v>0.8</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H15" si="13">SUM(B11:G11)</f>
-        <v>7.5</v>
+        <v>7.6</v>
       </c>
       <c r="J11">
         <f>B11-B10</f>
@@ -916,7 +916,7 @@
       </c>
       <c r="N11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="O11">
         <f t="shared" si="14"/>
@@ -940,14 +940,14 @@
         <v>1.4</v>
       </c>
       <c r="F12">
-        <v>1.2</v>
+        <v>1.45</v>
       </c>
       <c r="G12">
         <v>0.5</v>
       </c>
       <c r="H12">
         <f t="shared" si="13"/>
-        <v>8</v>
+        <v>8.25</v>
       </c>
       <c r="J12">
         <f t="shared" ref="J12:J15" si="15">B12-B11</f>
@@ -967,7 +967,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.14999999999999991</v>
       </c>
       <c r="O12">
         <f t="shared" si="14"/>
@@ -991,14 +991,14 @@
         <v>1.5</v>
       </c>
       <c r="F13">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="G13">
         <v>0.3</v>
       </c>
       <c r="H13">
         <f t="shared" si="13"/>
-        <v>8.6</v>
+        <v>9</v>
       </c>
       <c r="J13">
         <f t="shared" si="15"/>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.15000000000000013</v>
       </c>
       <c r="O13">
         <f t="shared" si="14"/>
@@ -1042,14 +1042,14 @@
         <v>1.5</v>
       </c>
       <c r="F14">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="G14">
         <v>0.3</v>
       </c>
       <c r="H14">
         <f t="shared" si="13"/>
-        <v>9.5</v>
+        <v>9.9</v>
       </c>
       <c r="J14">
         <f t="shared" si="15"/>
@@ -1093,14 +1093,14 @@
         <v>1.5</v>
       </c>
       <c r="F15">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="G15">
         <v>0.3</v>
       </c>
       <c r="H15">
         <f t="shared" si="13"/>
-        <v>9.5</v>
+        <v>9.9</v>
       </c>
       <c r="J15">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
Changes for the next release
</commit_message>
<xml_diff>
--- a/文档/产出平衡.xlsx
+++ b/文档/产出平衡.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB13E3A4-181C-467C-9A31-DDFF72B92EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FEFFE5-1DC3-4477-A439-1A2FC5A6E09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="2940" windowWidth="26205" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17295" yWindow="5235" windowWidth="20925" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="N12" sqref="N12:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -991,14 +991,14 @@
         <v>1.5</v>
       </c>
       <c r="F13">
-        <v>1.6</v>
+        <v>1.55</v>
       </c>
       <c r="G13">
         <v>0.3</v>
       </c>
       <c r="H13">
         <f t="shared" si="13"/>
-        <v>9</v>
+        <v>8.9500000000000011</v>
       </c>
       <c r="J13">
         <f t="shared" si="15"/>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="14"/>
-        <v>0.15000000000000013</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="O13">
         <f t="shared" si="14"/>
@@ -1039,17 +1039,17 @@
         <v>2</v>
       </c>
       <c r="E14">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="F14">
-        <v>1.6</v>
+        <v>1.55</v>
       </c>
       <c r="G14">
         <v>0.3</v>
       </c>
       <c r="H14">
         <f t="shared" si="13"/>
-        <v>9.9</v>
+        <v>9.9500000000000011</v>
       </c>
       <c r="J14">
         <f t="shared" si="15"/>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.10000000000000009</v>
       </c>
       <c r="N14">
         <f t="shared" si="14"/>
@@ -1090,17 +1090,17 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="F15">
-        <v>1.6</v>
+        <v>1.55</v>
       </c>
       <c r="G15">
         <v>0.3</v>
       </c>
       <c r="H15">
         <f t="shared" si="13"/>
-        <v>9.9</v>
+        <v>9.9500000000000011</v>
       </c>
       <c r="J15">
         <f t="shared" si="15"/>

</xml_diff>